<commit_message>
Fix production file errors
</commit_message>
<xml_diff>
--- a/production/Antdrive-top-pos.xlsx
+++ b/production/Antdrive-top-pos.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Antdrive\production\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{CF933CF3-ABDC-4792-A0B4-9ABE7FC407F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF543C1A-EF3E-4F43-AB72-46CD5DB32169}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1455" yWindow="4815" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="3270" yWindow="7170" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Antdrive-top-pos" sheetId="1" r:id="rId1"/>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -957,11 +957,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J1:P19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1099,7 +1099,7 @@
         <v>-52.704999999999998</v>
       </c>
       <c r="D8" s="3">
-        <v>270</v>
+        <v>90</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>1</v>
@@ -1235,7 +1235,7 @@
         <v>-53</v>
       </c>
       <c r="D16" s="3">
-        <v>90</v>
+        <v>270</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>1</v>
@@ -1252,7 +1252,7 @@
         <v>-45.085000000000001</v>
       </c>
       <c r="D17" s="3">
-        <v>0</v>
+        <v>270</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>1</v>
@@ -1269,7 +1269,7 @@
         <v>-44.637500000000003</v>
       </c>
       <c r="D18" s="3">
-        <v>0</v>
+        <v>270</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>1</v>

</xml_diff>